<commit_message>
Updated sections I had input incorrectly
</commit_message>
<xml_diff>
--- a/GF Done.xlsx
+++ b/GF Done.xlsx
@@ -723,8 +723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N367"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A352" workbookViewId="0">
-      <selection activeCell="P353" sqref="P353"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H224" sqref="H224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10318,7 +10318,7 @@
         <v>3</v>
       </c>
       <c r="H222" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I222" s="7" t="s">
         <v>18</v>
@@ -10362,7 +10362,7 @@
         <v>3</v>
       </c>
       <c r="H223" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I223" s="7" t="s">
         <v>18</v>
@@ -10828,7 +10828,7 @@
         <v>1</v>
       </c>
       <c r="H234" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I234" s="7" t="s">
         <v>18</v>
@@ -10870,7 +10870,7 @@
         <v>1</v>
       </c>
       <c r="H235" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I235" s="7" t="s">
         <v>18</v>
@@ -10912,7 +10912,7 @@
         <v>1</v>
       </c>
       <c r="H236" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I236" s="7" t="s">
         <v>18</v>
@@ -10996,7 +10996,7 @@
         <v>1</v>
       </c>
       <c r="H238" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I238" s="7" t="s">
         <v>18</v>
@@ -11038,7 +11038,7 @@
         <v>1</v>
       </c>
       <c r="H239" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I239" s="7" t="s">
         <v>18</v>
@@ -11080,7 +11080,7 @@
         <v>1</v>
       </c>
       <c r="H240" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I240" s="7" t="s">
         <v>18</v>
@@ -11122,7 +11122,7 @@
         <v>1</v>
       </c>
       <c r="H241" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I241" s="7" t="s">
         <v>18</v>
@@ -11164,7 +11164,7 @@
         <v>1</v>
       </c>
       <c r="H242" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I242" s="7" t="s">
         <v>18</v>
@@ -11206,7 +11206,7 @@
         <v>1</v>
       </c>
       <c r="H243" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I243" s="7" t="s">
         <v>18</v>
@@ -11248,7 +11248,7 @@
         <v>1</v>
       </c>
       <c r="H244" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I244" s="7" t="s">
         <v>18</v>
@@ -11290,7 +11290,7 @@
         <v>1</v>
       </c>
       <c r="H245" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I245" s="7" t="s">
         <v>18</v>
@@ -11332,7 +11332,7 @@
         <v>1</v>
       </c>
       <c r="H246" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I246" s="7" t="s">
         <v>18</v>
@@ -11374,7 +11374,7 @@
         <v>1</v>
       </c>
       <c r="H247" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I247" s="7" t="s">
         <v>18</v>
@@ -11416,7 +11416,7 @@
         <v>1</v>
       </c>
       <c r="H248" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I248" s="7" t="s">
         <v>18</v>
@@ -11458,7 +11458,7 @@
         <v>1</v>
       </c>
       <c r="H249" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I249" s="7" t="s">
         <v>18</v>
@@ -11500,7 +11500,7 @@
         <v>1</v>
       </c>
       <c r="H250" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I250" s="7" t="s">
         <v>18</v>
@@ -11542,7 +11542,7 @@
         <v>1</v>
       </c>
       <c r="H251" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I251" s="7" t="s">
         <v>18</v>
@@ -11584,7 +11584,7 @@
         <v>1</v>
       </c>
       <c r="H252" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I252" s="7" t="s">
         <v>18</v>
@@ -11626,7 +11626,7 @@
         <v>1</v>
       </c>
       <c r="H253" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I253" s="7" t="s">
         <v>18</v>
@@ -11710,7 +11710,7 @@
         <v>1</v>
       </c>
       <c r="H255" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I255" s="7" t="s">
         <v>18</v>
@@ -11752,7 +11752,7 @@
         <v>1</v>
       </c>
       <c r="H256" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I256" s="7" t="s">
         <v>18</v>
@@ -11794,7 +11794,7 @@
         <v>1</v>
       </c>
       <c r="H257" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I257" s="7" t="s">
         <v>18</v>
@@ -11836,7 +11836,7 @@
         <v>1</v>
       </c>
       <c r="H258" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I258" s="7" t="s">
         <v>18</v>
@@ -11878,7 +11878,7 @@
         <v>1</v>
       </c>
       <c r="H259" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I259" s="7" t="s">
         <v>25</v>
@@ -11920,7 +11920,7 @@
         <v>1</v>
       </c>
       <c r="H260" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I260" s="7" t="s">
         <v>18</v>
@@ -11962,7 +11962,7 @@
         <v>1</v>
       </c>
       <c r="H261" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I261" s="7" t="s">
         <v>18</v>
@@ -12004,7 +12004,7 @@
         <v>1</v>
       </c>
       <c r="H262" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I262" s="7" t="s">
         <v>18</v>
@@ -12046,7 +12046,7 @@
         <v>1</v>
       </c>
       <c r="H263" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I263" s="7" t="s">
         <v>18</v>
@@ -12088,7 +12088,7 @@
         <v>1</v>
       </c>
       <c r="H264" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I264" s="7" t="s">
         <v>18</v>
@@ -12172,7 +12172,7 @@
         <v>1</v>
       </c>
       <c r="H266" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I266" s="7" t="s">
         <v>18</v>
@@ -12214,7 +12214,7 @@
         <v>1</v>
       </c>
       <c r="H267" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I267" s="7" t="s">
         <v>18</v>
@@ -12256,7 +12256,7 @@
         <v>1</v>
       </c>
       <c r="H268" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I268" s="7" t="s">
         <v>18</v>
@@ -12298,7 +12298,7 @@
         <v>1</v>
       </c>
       <c r="H269" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I269" s="7" t="s">
         <v>18</v>
@@ -12340,7 +12340,7 @@
         <v>1</v>
       </c>
       <c r="H270" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I270" s="7" t="s">
         <v>18</v>
@@ -12382,7 +12382,7 @@
         <v>1</v>
       </c>
       <c r="H271" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I271" s="7" t="s">
         <v>18</v>
@@ -12424,7 +12424,7 @@
         <v>1</v>
       </c>
       <c r="H272" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I272" s="7" t="s">
         <v>18</v>
@@ -12466,7 +12466,7 @@
         <v>1</v>
       </c>
       <c r="H273" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I273" s="7" t="s">
         <v>18</v>
@@ -12508,7 +12508,7 @@
         <v>1</v>
       </c>
       <c r="H274" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I274" s="7" t="s">
         <v>18</v>
@@ -12550,7 +12550,7 @@
         <v>1</v>
       </c>
       <c r="H275" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I275" s="7" t="s">
         <v>18</v>
@@ -12592,7 +12592,7 @@
         <v>1</v>
       </c>
       <c r="H276" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I276" s="7" t="s">
         <v>18</v>
@@ -12634,7 +12634,7 @@
         <v>1</v>
       </c>
       <c r="H277" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I277" s="7" t="s">
         <v>18</v>
@@ -12928,7 +12928,7 @@
         <v>1</v>
       </c>
       <c r="H284" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I284" s="7" t="s">
         <v>18</v>
@@ -13012,7 +13012,7 @@
         <v>1</v>
       </c>
       <c r="H286" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I286" s="7" t="s">
         <v>18</v>
@@ -13054,7 +13054,7 @@
         <v>1</v>
       </c>
       <c r="H287" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I287" s="7" t="s">
         <v>18</v>
@@ -13096,7 +13096,7 @@
         <v>1</v>
       </c>
       <c r="H288" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I288" s="7" t="s">
         <v>18</v>
@@ -13180,7 +13180,7 @@
         <v>1</v>
       </c>
       <c r="H290" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I290" s="7" t="s">
         <v>25</v>
@@ -13390,7 +13390,7 @@
         <v>1</v>
       </c>
       <c r="H295" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I295" s="7" t="s">
         <v>18</v>
@@ -13432,7 +13432,7 @@
         <v>1</v>
       </c>
       <c r="H296" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I296" s="7" t="s">
         <v>18</v>
@@ -13474,7 +13474,7 @@
         <v>1</v>
       </c>
       <c r="H297" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I297" s="7" t="s">
         <v>18</v>
@@ -13516,7 +13516,7 @@
         <v>1</v>
       </c>
       <c r="H298" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I298" s="7" t="s">
         <v>18</v>
@@ -13726,7 +13726,7 @@
         <v>1</v>
       </c>
       <c r="H303" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I303" s="7" t="s">
         <v>18</v>
@@ -13768,7 +13768,7 @@
         <v>1</v>
       </c>
       <c r="H304" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I304" s="7" t="s">
         <v>18</v>
@@ -13810,7 +13810,7 @@
         <v>1</v>
       </c>
       <c r="H305" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I305" s="7" t="s">
         <v>18</v>
@@ -13894,7 +13894,7 @@
         <v>1</v>
       </c>
       <c r="H307" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I307" s="7" t="s">
         <v>18</v>
@@ -14104,7 +14104,7 @@
         <v>1</v>
       </c>
       <c r="H312" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I312" s="7" t="s">
         <v>25</v>
@@ -14230,7 +14230,7 @@
         <v>1</v>
       </c>
       <c r="H315" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I315" s="7" t="s">
         <v>18</v>
@@ -14272,7 +14272,7 @@
         <v>1</v>
       </c>
       <c r="H316" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I316" s="7" t="s">
         <v>18</v>
@@ -14314,7 +14314,7 @@
         <v>1</v>
       </c>
       <c r="H317" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I317" s="7" t="s">
         <v>18</v>
@@ -14356,7 +14356,7 @@
         <v>1</v>
       </c>
       <c r="H318" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I318" s="7" t="s">
         <v>18</v>
@@ -14398,7 +14398,7 @@
         <v>1</v>
       </c>
       <c r="H319" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I319" s="7" t="s">
         <v>18</v>
@@ -14440,7 +14440,7 @@
         <v>1</v>
       </c>
       <c r="H320" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I320" s="7" t="s">
         <v>18</v>
@@ -14482,7 +14482,7 @@
         <v>1</v>
       </c>
       <c r="H321" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I321" s="7" t="s">
         <v>18</v>
@@ -14524,7 +14524,7 @@
         <v>1</v>
       </c>
       <c r="H322" s="11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I322" s="11" t="s">
         <v>25</v>
@@ -14610,7 +14610,7 @@
         <v>1</v>
       </c>
       <c r="H324" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I324" s="7" t="s">
         <v>18</v>
@@ -14698,7 +14698,7 @@
         <v>1</v>
       </c>
       <c r="H326" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I326" s="7" t="s">
         <v>18</v>
@@ -14742,7 +14742,7 @@
         <v>1</v>
       </c>
       <c r="H327" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I327" s="7" t="s">
         <v>18</v>
@@ -14830,7 +14830,7 @@
         <v>1</v>
       </c>
       <c r="H329" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I329" s="7" t="s">
         <v>18</v>
@@ -14962,7 +14962,7 @@
         <v>1</v>
       </c>
       <c r="H332" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I332" s="7" t="s">
         <v>18</v>
@@ -15226,7 +15226,7 @@
         <v>1</v>
       </c>
       <c r="H338" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I338" s="7" t="s">
         <v>18</v>
@@ -15268,7 +15268,7 @@
         <v>1</v>
       </c>
       <c r="H339" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I339" s="7" t="s">
         <v>18</v>
@@ -15310,7 +15310,7 @@
         <v>1</v>
       </c>
       <c r="H340" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I340" s="7" t="s">
         <v>18</v>
@@ -15352,7 +15352,7 @@
         <v>1</v>
       </c>
       <c r="H341" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I341" s="7" t="s">
         <v>18</v>
@@ -15940,7 +15940,7 @@
         <v>1</v>
       </c>
       <c r="H355" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I355" s="7" t="s">
         <v>18</v>
@@ -15982,7 +15982,7 @@
         <v>1</v>
       </c>
       <c r="H356" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I356" s="7" t="s">
         <v>18</v>
@@ -16024,7 +16024,7 @@
         <v>1</v>
       </c>
       <c r="H357" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I357" s="7" t="s">
         <v>18</v>
@@ -16318,7 +16318,7 @@
         <v>1</v>
       </c>
       <c r="H364" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I364" s="7" t="s">
         <v>18</v>
@@ -16360,7 +16360,7 @@
         <v>1</v>
       </c>
       <c r="H365" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I365" s="7" t="s">
         <v>18</v>
@@ -16444,7 +16444,7 @@
         <v>1</v>
       </c>
       <c r="H367" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I367" s="11" t="s">
         <v>18</v>

</xml_diff>